<commit_message>
updated to round 4
</commit_message>
<xml_diff>
--- a/result_list_round_3.xlsx
+++ b/result_list_round_3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,825 +463,425 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Big Bam Theory (6)</t>
+          <t>Big Bam Theory (0)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Team Becks (3)</t>
+          <t>Los Angeles Ballerz (0)</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Big Bam Theory</t>
+          <t>Not Determined</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Team Becks</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GIDDEY UPS - MAILMAN 2.0 (1)</t>
+          <t>Team Wallace (0)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Los Angeles Ballerz (9)</t>
+          <t>Wham Bam Thankyou Ma’am (0)</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Los Angeles Ballerz</t>
+          <t>Not Determined</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>GIDDEY UPS - MAILMAN 2.0</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Harrison the league (3)</t>
+          <t>Funghi Curry (0)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Wham Bam Thankyou Ma’am (7)</t>
+          <t>Who what where when Kawhi (0)</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Wham Bam Thankyou Ma’am</t>
+          <t>Not Determined</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Harrison the league</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Brooks, Crooks and Sooks (2)</t>
+          <t>Josh Kiddey (0)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Team Wallace (8)</t>
+          <t>TankCity Unicorns (0)</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Team Wallace</t>
+          <t>Not Determined</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Brooks, Crooks and Sooks</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Keyonte George Costanza (5)</t>
+          <t>Daryl's Discount Dimes (0)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Who what where when Kawhi (6)</t>
+          <t>Flex n Affect (0)</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Who what where when Kawhi</t>
+          <t>Not Determined</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Keyonte George Costanza</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Funghi Curry (7)</t>
+          <t>Luka Warm (0)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ol' Dirty Baskets (4)</t>
+          <t>The Chet Code (0)</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Funghi Curry</t>
+          <t>Not Determined</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Ol' Dirty Baskets</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>OKC-OOPS (4)</t>
+          <t>Atlanta Waivers (0)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>TankCity Unicorns (6)</t>
+          <t>Scottie Pippings (0)</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>TankCity Unicorns</t>
+          <t>Not Determined</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>OKC-OOPS</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Josh Kiddey (6)</t>
+          <t>Jaylen CAN go left! (0)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Team irwin (3)</t>
+          <t>Mile High Mutombo's (0)</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Josh Kiddey</t>
+          <t>Not Determined</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Team irwin</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Flex n Affect (6)</t>
+          <t>GOLD COAST GREMLINS (0)</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Jimmy Brings (3)</t>
+          <t>Little Buff Boys (0)</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Flex n Affect</t>
+          <t>Not Determined</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Jimmy Brings</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Daryl's Discount Dimes (8)</t>
+          <t>Darwin Esky (0)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Minnesota Lumberjacks (3)</t>
+          <t>Diamond D Dynasty (0)</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Daryl's Discount Dimes</t>
+          <t>Not Determined</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Minnesota Lumberjacks</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ANUS BLEACHING SEA LIONS (2)</t>
+          <t>OG Wan Unobi (0)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>The Chet Code (8)</t>
+          <t>The Great Hali (0)</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>The Chet Code</t>
+          <t>Not Determined</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>ANUS BLEACHING SEA LIONS</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Balls Deep (5)</t>
+          <t>BIG BULLS (0)</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Luka Warm (6)</t>
+          <t>The Hairy Skips (0)</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Luka Warm</t>
+          <t>Not Determined</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Balls Deep</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Gladysisahoe Dazz (5)</t>
+          <t>Ja 'his real name is Clarence' (0)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Scottie Pippings (6)</t>
+          <t>The Book of Irving (0)</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Scottie Pippings</t>
+          <t>Not Determined</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Gladysisahoe Dazz</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Atlanta Waivers (6)</t>
+          <t>Red Dragons (0)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Bronsexual Lebrolites (5)</t>
+          <t>Townsville Crocs (0)</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Atlanta Waivers</t>
+          <t>Not Determined</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Bronsexual Lebrolites</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Jaylen CAN go left! (6)</t>
+          <t>Kingcalvin (0)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>War Grimes in Garza (5)</t>
+          <t>The Flaming Galahs (0)</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Jaylen CAN go left!</t>
+          <t>Not Determined</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>War Grimes in Garza</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Boots Manuva (4)</t>
+          <t>Boomtown Bulls (0)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Mile High Mutombo's (6)</t>
+          <t>Dort Stop Believin (0)</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Mile High Mutombo's</t>
+          <t>Not Determined</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Boots Manuva</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Donnys Beans (4)</t>
+          <t>Don't Go Blakin My Heart (0)</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Little Buff Boys (6)</t>
+          <t>James and the Giant Overreach (0)</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Little Buff Boys</t>
+          <t>Not Determined</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Donnys Beans</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Globetrotter Gunts (3)</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>GOLD COAST GREMLINS (7)</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>1</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>GOLD COAST GREMLINS</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Globetrotter Gunts</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>BigZ Spurs (4)</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Diamond D Dynasty (7)</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Diamond D Dynasty</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>BigZ Spurs</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Darwin Esky (8)</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Moves Like Agger (0)</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>3</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Darwin Esky</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Moves Like Agger</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>SavedByTheKelle (5)</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>The Great Hali (6)</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>The Great Hali</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>SavedByTheKelle</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>OG Wan Unobi (5)</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>ROUdiamondGH (4)</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>2</v>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>OG Wan Unobi</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>ROUdiamondGH</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Bank Town Squids (5)</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>BIG BULLS (6)</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>BIG BULLS</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Bank Town Squids</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>ChixnGrog (3)</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>The Hairy Skips (8)</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>The Hairy Skips</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>ChixnGrog</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Seattle SuperChronics (5)</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>The Book of Irving (6)</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>1</v>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>The Book of Irving</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Seattle SuperChronics</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Ja 'his real name is Clarence' (6)</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Panania Rockets (3)</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>2</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Ja 'his real name is Clarence'</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Panania Rockets</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Houston Mob Squad (5)</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Townsville Crocs (6)</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>1</v>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Townsville Crocs</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Houston Mob Squad</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Indiana Monstars (1)</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Red Dragons (9)</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Red Dragons</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Indiana Monstars</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Kingcalvin (8)</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Signature Moves (3)</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Kingcalvin</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Signature Moves</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Ja Raffe (3)</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>The Flaming Galahs (8)</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>0</v>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>The Flaming Galahs</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Ja Raffe</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Dort Stop Believin (7)</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Valentuna Sandwhich (2)</t>
-        </is>
-      </c>
-      <c r="C32" t="n">
-        <v>2</v>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Dort Stop Believin</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Valentuna Sandwhich</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Boomtown Bulls (8)</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Don't Go Blakin My Heart (2)</t>
-        </is>
-      </c>
-      <c r="C33" t="n">
-        <v>1</v>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Boomtown Bulls</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Don't Go Blakin My Heart</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Duncans Donuts (4)</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>James and the Giant Overreach (5)</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>2</v>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>James and the Giant Overreach</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>Duncans Donuts</t>
+          <t>Not Determined</t>
         </is>
       </c>
     </row>

</xml_diff>